<commit_message>
Feito do Exercicio 1 até 4
</commit_message>
<xml_diff>
--- a/exercicios_crud_mysql.xlsx
+++ b/exercicios_crud_mysql.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\teste\MySQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\MySQL\Exercícios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD4C5728-3341-4240-B8E8-7416626F4EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76114E49-D5AC-44F6-AAC9-E809BEC0FCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="A2:G22"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -546,7 +546,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +568,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Feito do Exercício 5 ao 7
</commit_message>
<xml_diff>
--- a/exercicios_crud_mysql.xlsx
+++ b/exercicios_crud_mysql.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\MySQL\Exercícios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\teste\MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76114E49-D5AC-44F6-AAC9-E809BEC0FCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE701D-0792-4977-A5B1-7D04185265AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>21</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,7 +590,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Feito Exercicio 8 e 9
</commit_message>
<xml_diff>
--- a/exercicios_crud_mysql.xlsx
+++ b/exercicios_crud_mysql.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\teste\MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE701D-0792-4977-A5B1-7D04185265AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE42AC62-744E-4F13-9FC3-5BB6ADE91DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,7 +623,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Feito Exercício 11 ao 15 || Finalizado
</commit_message>
<xml_diff>
--- a/exercicios_crud_mysql.xlsx
+++ b/exercicios_crud_mysql.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\teste\MySQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programação\MySQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C548BD-AD26-47F9-934C-FF3C0F96BFD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDDC7BC-B51D-4A79-861D-FAEE6547DE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>